<commit_message>
some updates to make reservation..To be Continued
</commit_message>
<xml_diff>
--- a/System development files/Operation Contracts.xlsx
+++ b/System development files/Operation Contracts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
   <si>
     <t>Operation:</t>
   </si>
@@ -47,51 +47,21 @@
     <t>a Table instance is created</t>
   </si>
   <si>
-    <t>a reservation was made</t>
-  </si>
-  <si>
     <t>table is reserved and not available for others</t>
   </si>
   <si>
     <t>In case of preorder an inactive order has been created</t>
   </si>
   <si>
-    <t>insertTableNo(tableNo)</t>
-  </si>
-  <si>
     <t>Reservatin ha started</t>
   </si>
   <si>
-    <t>table number was inserted</t>
-  </si>
-  <si>
     <t>The reservation procedure ha started</t>
   </si>
   <si>
     <t>findTableByNo(tableNo)</t>
   </si>
   <si>
-    <t>The system starts to search for the table</t>
-  </si>
-  <si>
-    <t>searchTable(tableNo)</t>
-  </si>
-  <si>
-    <t>A request to find a table was made</t>
-  </si>
-  <si>
-    <t>Database finds requested table</t>
-  </si>
-  <si>
-    <t>getTable(tableNo)</t>
-  </si>
-  <si>
-    <t>Database searched for the table</t>
-  </si>
-  <si>
-    <t>Table is returned</t>
-  </si>
-  <si>
     <t>checkIfExists()</t>
   </si>
   <si>
@@ -126,6 +96,21 @@
   </si>
   <si>
     <t>A confirmation message has been printed out</t>
+  </si>
+  <si>
+    <t>enterTableNo(tableNo)</t>
+  </si>
+  <si>
+    <t>table number was entered</t>
+  </si>
+  <si>
+    <t>The system finds the table</t>
+  </si>
+  <si>
+    <t>New reservation instance is created</t>
+  </si>
+  <si>
+    <t>New reservation is saved in the database</t>
   </si>
 </sst>
 </file>
@@ -479,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +476,7 @@
     <col min="2" max="2" width="59.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -507,53 +492,47 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="1"/>
-      <c r="H5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -561,35 +540,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
     </row>
@@ -598,7 +577,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -614,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -622,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +621,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -658,7 +637,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -666,7 +645,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -686,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -702,7 +681,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -710,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -730,7 +709,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -754,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -774,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -790,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -798,7 +777,7 @@
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -813,115 +792,22 @@
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="4"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="4"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="1"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="4"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A68:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B46:B47"/>
+  <mergeCells count="14">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A60:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B22:B23"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B46:B47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Some comments on SSD and Operation Contracts
</commit_message>
<xml_diff>
--- a/System development files/Operation Contracts.xlsx
+++ b/System development files/Operation Contracts.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Desktop w10\Semester 2\SecondSemesterProject\Github\Semester2\dmai0914-semester2-finalProject-group3\System development files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -269,17 +264,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -290,9 +282,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -562,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -635,10 +630,10 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -649,54 +644,54 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="8"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="8"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="9"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="9"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="9"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="9"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -753,62 +748,62 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
+      <c r="A14" s="5"/>
+      <c r="B14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="9"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="9"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -859,7 +854,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -871,50 +866,50 @@
       <c r="E20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="7" t="s">
+      <c r="G20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="1"/>
-      <c r="D21" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="8"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="D22" s="3" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="9"/>
+      <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="8"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="9"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="9"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -923,8 +918,8 @@
       <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -943,7 +938,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -951,16 +946,16 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="9"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -987,7 +982,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -995,16 +990,16 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
+      <c r="A37" s="5"/>
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="9"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="9"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1031,7 +1026,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -1039,16 +1034,16 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
+      <c r="A45" s="5"/>
       <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="9"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="9"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
@@ -1075,7 +1070,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -1083,31 +1078,25 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="5"/>
       <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="9"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-      <c r="B55" s="4"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B22:B23"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="A28:A31"/>
@@ -1116,12 +1105,18 @@
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update ChoosenTableDialog and fully dressed
</commit_message>
<xml_diff>
--- a/System development files/Operation Contracts.xlsx
+++ b/System development files/Operation Contracts.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="48">
   <si>
     <t>Operation:</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Post conditions:</t>
   </si>
   <si>
-    <t>makeReservation(customersName,phoneNo,date,preorder)</t>
-  </si>
-  <si>
     <t>Make reservation</t>
   </si>
   <si>
@@ -108,43 +105,13 @@
     <t>New reservation is saved in the database</t>
   </si>
   <si>
-    <t>makeOrder(table:Table, waiter:Stuff)</t>
-  </si>
-  <si>
     <t>Make order</t>
   </si>
   <si>
-    <t>Table is created, Stuff is created</t>
-  </si>
-  <si>
-    <t>Order object is created and accosiated with table</t>
-  </si>
-  <si>
-    <t>Stuff object associated with the order object</t>
-  </si>
-  <si>
     <t>insertMerchandise(product:Merchandise,quantity)</t>
   </si>
   <si>
     <t xml:space="preserve">Order object is created </t>
-  </si>
-  <si>
-    <t>OrderLine is created and associated with the order</t>
-  </si>
-  <si>
-    <t>Merchandise objects associated with the OrderLine</t>
-  </si>
-  <si>
-    <t>makePayment(order:Order)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Order is created </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retrieve total from order obejct </t>
-  </si>
-  <si>
-    <t>Return information about the order</t>
   </si>
   <si>
     <t>createMerchandise(name, price, type)</t>
@@ -173,6 +140,31 @@
   </si>
   <si>
     <t>Item is updated.</t>
+  </si>
+  <si>
+    <t>makeOrder(cprNo:int, isactive: boolean)</t>
+  </si>
+  <si>
+    <t>Stuff is created</t>
+  </si>
+  <si>
+    <t>Order object is created and accosiated with reservation
+and waiter</t>
+  </si>
+  <si>
+    <t>makeReservation(customersName,phoneNo,date)</t>
+  </si>
+  <si>
+    <t>findMerchandise(name:String)</t>
+  </si>
+  <si>
+    <t>Obejct returns found merchandise</t>
+  </si>
+  <si>
+    <t>Merchandise found, order object created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obejct Merchandise accosiated with obejct order </t>
   </si>
 </sst>
 </file>
@@ -260,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -273,6 +265,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -282,8 +283,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,7 +572,7 @@
   <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H23"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,7 +581,7 @@
     <col min="2" max="2" width="54.140625" customWidth="1"/>
     <col min="3" max="3" width="3.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.140625" customWidth="1"/>
     <col min="6" max="6" width="2.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="40.5703125" bestFit="1" customWidth="1"/>
@@ -588,19 +592,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -608,19 +612,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -628,83 +632,81 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>45</v>
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="12"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="9"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="9"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="9"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -712,19 +714,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -732,91 +734,89 @@
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>48</v>
+      <c r="G12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="1"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="9"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="8"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="5"/>
-      <c r="E16" s="9"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -824,13 +824,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -838,95 +838,95 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="1"/>
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="9"/>
-      <c r="D22" s="5" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="D22" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="9"/>
-      <c r="D23" s="5"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="D23" s="7"/>
       <c r="E23" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
-      <c r="E24" s="9"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,35 +934,35 @@
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -970,7 +970,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,35 +978,35 @@
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="8"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="7"/>
+      <c r="B39" s="8"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1014,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1022,35 +1022,35 @@
         <v>2</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="1"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="7"/>
+      <c r="B46" s="8"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="9"/>
+      <c r="A47" s="7"/>
+      <c r="B47" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1058,7 +1058,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1066,37 +1066,43 @@
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="1"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="9"/>
+      <c r="A54" s="7"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="9"/>
+      <c r="A55" s="7"/>
+      <c r="B55" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="D4:D7"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="A28:A31"/>
@@ -1105,18 +1111,12 @@
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="A44:A47"/>
     <mergeCell ref="B46:B47"/>
-    <mergeCell ref="D4:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D22:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The latest version for Richard
We have to add there some diagrams but we will make it tommorow, so you
can checkmistakes
</commit_message>
<xml_diff>
--- a/System development files/Operation Contracts.xlsx
+++ b/System development files/Operation Contracts.xlsx
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -232,6 +232,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -240,27 +246,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -269,11 +254,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,7 +565,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -557,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,52 +652,52 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="20" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="15"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="11"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="17"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="21"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="21"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="6"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -736,7 +754,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -748,48 +766,48 @@
       <c r="E12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="1"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="11"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="13"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="13"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="12"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="24"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D16" s="9"/>
-      <c r="E16" s="13"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -852,163 +870,165 @@
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="16"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="D21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="D22" s="5" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="16"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="8"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="16"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="11"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
-      <c r="B29" s="17"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
-      <c r="B30" s="17"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="11"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="11"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
-      <c r="B37" s="17"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="11"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
-      <c r="B43" s="16"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="11"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
-      <c r="B44" s="16"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="17"/>
-      <c r="B46" s="17"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="16"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="16"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="16"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="11"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="16"/>
+      <c r="A53" s="12"/>
+      <c r="B53" s="11"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="9">
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
     <mergeCell ref="A4:A7"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="B14:B15"/>
@@ -1016,11 +1036,8 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G4:G7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="H12:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>